<commit_message>
GiovanniPC: Jueves 3 de Febrero de 2016
</commit_message>
<xml_diff>
--- a/docs/Encuestas Sagrado/Usuarios.xlsx
+++ b/docs/Encuestas Sagrado/Usuarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="11655" windowHeight="2835" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="11655" windowHeight="2835" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Usuario1" sheetId="1" r:id="rId1"/>
@@ -3285,8 +3285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:K237"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A35" sqref="A34:A35"/>
+    <sheetView topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7337,7 +7337,7 @@
   <dimension ref="B1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7352,7 +7352,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="2" spans="2:4" ht="30">
+    <row r="2" spans="2:4">
       <c r="B2" s="2">
         <v>2</v>
       </c>
@@ -7363,7 +7363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="30">
+    <row r="3" spans="2:4">
       <c r="B3" s="2">
         <v>5</v>
       </c>
@@ -7396,7 +7396,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="30">
+    <row r="6" spans="2:4">
       <c r="B6" s="2">
         <v>8</v>
       </c>
@@ -7418,7 +7418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="30">
+    <row r="8" spans="2:4">
       <c r="B8" s="2">
         <v>15</v>
       </c>
@@ -7429,7 +7429,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="30">
+    <row r="9" spans="2:4">
       <c r="B9" s="2">
         <v>18</v>
       </c>
@@ -7440,7 +7440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="60">
+    <row r="10" spans="2:4">
       <c r="B10" s="2">
         <v>19</v>
       </c>
@@ -7482,11 +7482,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K204"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K204"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
@@ -14637,8 +14641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>